<commit_message>
force intervals calculations added: 6799 frames
</commit_message>
<xml_diff>
--- a/results_test/ch2_permation_residue_comb.xlsx
+++ b/results_test/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,27 +458,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 130, 455, 780</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6727</t>
+          <t>5178, 5582</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 455, 780, 1105</t>
+          <t>98, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>5552</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 130, 423, 1073</t>
+          <t>130, 780, 780</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,25 +511,385 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6670</t>
+          <t>3171</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>98, 130, 748, 748</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3631</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>98, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3666</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>130, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5131</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>98, 130, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4415</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>423, 1073, 1105, SF, SF</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4994</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>130, 455, 748, 780</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5269</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>455, 748, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>5677</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>423, 748, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1105, 1105</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5331, 5433</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>423, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>455</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5886</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>98, 130, 455, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6016</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6202</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>130, 455, SF</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6425</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>98, 130, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6488</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>130, 455, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>98, 780, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>98, 130, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>6727</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>130, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>98, 98, 455, 455</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="inlineStr">
         <is>
           <t>455</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
Change com of atoms to mid dist atoms
</commit_message>
<xml_diff>
--- a/results_test/ch2_permation_residue_comb.xlsx
+++ b/results_test/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,23 +502,23 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 780</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3171</t>
+          <t>3171, 3666</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>98, 130, 748, 748</t>
+          <t>98, 130, 748, 780</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -538,7 +538,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>98, 780, 1105</t>
+          <t>130, 455, 748, 1073</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -546,39 +546,39 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3666</t>
+          <t>5131</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>130, 455, 748, 1073</t>
+          <t>98, 130, 455, 1073</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>4416, 6489</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>98, 130, 1073, SF</t>
+          <t>423, 1073, 1105, SF, SF</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -586,19 +586,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4415</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>423, 1073, 1105, SF, SF</t>
+          <t>130, 455, 748, 780</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -606,19 +606,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4994</t>
+          <t>5269</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>130, 455, 748, 780</t>
+          <t>455, 748, 1073, 1105</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -626,19 +626,19 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5269</t>
+          <t>5399</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>455, 748, 1073, 1105</t>
+          <t>423, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -646,59 +646,59 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>5677</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073</t>
+          <t>423, 748, 1073, 1105</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>1105, 1105</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5677</t>
+          <t>5331, 5433</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>423, 748, 1073, 1105</t>
+          <t>423, 455, 748, 1073</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1105, 1105</t>
+          <t>455</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5331, 5433</t>
+          <t>5886</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>423, 455, 748, 1073</t>
+          <t>98, 130, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -706,19 +706,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5886</t>
+          <t>6017</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>98, 130, 455, 780, 1073</t>
+          <t>130, 423, 748, 1073, SF</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -731,14 +731,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6016</t>
+          <t>6202</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>130, 423, 748, 1073, SF</t>
+          <t>98, 130, 455</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -751,14 +751,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6202</t>
+          <t>6427</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>130, 455, SF</t>
+          <t>130, 455, 780, 1073</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -771,14 +771,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6425</t>
+          <t>6562</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>98, 130, 780, 1073</t>
+          <t>130, 780, 780, 1073</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -786,19 +786,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6488</t>
+          <t>6359</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>130, 455, 780, 1105</t>
+          <t>98, 130, 130, 455, 780</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -811,14 +811,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>98, 780, 780, 1073</t>
+          <t>98, 130, 423, 1073</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -826,19 +826,19 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6359</t>
+          <t>6670</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>98, 130, 130, 455, 780</t>
+          <t>98, 98, 455, 455</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -846,50 +846,10 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>455</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
-        <is>
-          <t>6727</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>130, 130, 423, 1073</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>98, 98, 455, 455</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>455</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>